<commit_message>
feat: add groups for excel preset
</commit_message>
<xml_diff>
--- a/assets/signaturepresets/preset1.xlsx
+++ b/assets/signaturepresets/preset1.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\var\www\html\ruestzeit-anmeldung\assets\signaturepresets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{E4178966-DCA8-45FB-A458-21E3499A89A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B765F4B1-29A0-4AFC-85B4-D01FD9C91DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Tabelle1!$8:$9</definedName>
@@ -787,7 +785,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -988,32 +986,4 @@
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
 </file>
</xml_diff>